<commit_message>
cx_Freeze compile with database: death to Python2.7
</commit_message>
<xml_diff>
--- a/python3.6/PIP_GEN_id-0/Parts - Consoles.xlsx
+++ b/python3.6/PIP_GEN_id-0/Parts - Consoles.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="110">
   <si>
     <t>RecordID</t>
   </si>
@@ -349,10 +349,10 @@
     <t>20171005</t>
   </si>
   <si>
-    <t>From chaos, springs new beginnings!</t>
-  </si>
-  <si>
-    <t>LOKI</t>
+    <t>Order from chaos</t>
+  </si>
+  <si>
+    <t>id-0</t>
   </si>
   <si>
     <t>REV 1</t>
@@ -364,9 +364,6 @@
     <t>Created arrays for variables</t>
   </si>
   <si>
-    <t>id-0</t>
-  </si>
-  <si>
     <t>REV 2</t>
   </si>
   <si>
@@ -421,7 +418,7 @@
     <t>About done</t>
   </si>
   <si>
-    <t>REV</t>
+    <t>REV 8</t>
   </si>
   <si>
     <t>20180228</t>
@@ -430,7 +427,19 @@
     <t>Migrated to Python3.6.4</t>
   </si>
   <si>
-    <t>Let justice be done, though the heavens fall!</t>
+    <t>REV 9</t>
+  </si>
+  <si>
+    <t>20180307</t>
+  </si>
+  <si>
+    <t>Test build with cx_Freeze5.1.1</t>
+  </si>
+  <si>
+    <t>REV x.x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fiat justitia ruat caelum </t>
   </si>
 </sst>
 </file>
@@ -1070,7 +1079,7 @@
         <v>76</v>
       </c>
       <c r="BA2" s="2" t="n">
-        <v>43159.57195233466</v>
+        <v>43166.75561099128</v>
       </c>
     </row>
   </sheetData>
@@ -1084,7 +1093,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1092,9 +1101,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="8.4"/>
+    <col customWidth="1" max="1" min="1" width="10.8"/>
     <col customWidth="1" max="2" min="2" width="12"/>
-    <col customWidth="1" max="3" min="3" width="56.4"/>
+    <col customWidth="1" max="3" min="3" width="46.8"/>
     <col customWidth="1" max="4" min="4" width="7.199999999999999"/>
   </cols>
   <sheetData>
@@ -1123,119 +1132,133 @@
         <v>83</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
         <v>85</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>86</v>
       </c>
-      <c r="C3" t="s">
-        <v>87</v>
-      </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" t="s">
         <v>88</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>89</v>
       </c>
-      <c r="C4" t="s">
-        <v>90</v>
-      </c>
       <c r="D4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" t="s">
         <v>91</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>92</v>
       </c>
-      <c r="C5" t="s">
-        <v>93</v>
-      </c>
       <c r="D5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" t="s">
         <v>94</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>95</v>
       </c>
-      <c r="C6" t="s">
-        <v>96</v>
-      </c>
       <c r="D6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" t="s">
         <v>97</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>98</v>
       </c>
-      <c r="C7" t="s">
-        <v>99</v>
-      </c>
       <c r="D7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" t="s">
         <v>100</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>101</v>
       </c>
-      <c r="C8" t="s">
-        <v>102</v>
-      </c>
       <c r="D8" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" t="s">
         <v>103</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>104</v>
       </c>
-      <c r="C9" t="s">
-        <v>105</v>
-      </c>
       <c r="D9" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>103</v>
-      </c>
-      <c r="B10" s="2" t="n">
-        <v>43159.57186623513</v>
+        <v>105</v>
+      </c>
+      <c r="B10" t="s">
+        <v>106</v>
       </c>
       <c r="C10" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D10" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>43166.75549595193</v>
+      </c>
+      <c r="C11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Need to finish streamlining code
</commit_message>
<xml_diff>
--- a/python3.6/PIP_GEN_id-0/Parts - Consoles.xlsx
+++ b/python3.6/PIP_GEN_id-0/Parts - Consoles.xlsx
@@ -343,7 +343,7 @@
     <t>PIP_Generator</t>
   </si>
   <si>
-    <t>REV 0</t>
+    <t>V.0</t>
   </si>
   <si>
     <t>20171005</t>
@@ -355,7 +355,7 @@
     <t>id-0</t>
   </si>
   <si>
-    <t>REV 1</t>
+    <t>V.1</t>
   </si>
   <si>
     <t>20171205</t>
@@ -364,7 +364,7 @@
     <t>Created arrays for variables</t>
   </si>
   <si>
-    <t>REV 2</t>
+    <t>V.2</t>
   </si>
   <si>
     <t>20171206</t>
@@ -373,7 +373,7 @@
     <t>Added time stamping</t>
   </si>
   <si>
-    <t>REV 3</t>
+    <t>V.3</t>
   </si>
   <si>
     <t>20171207</t>
@@ -382,7 +382,7 @@
     <t>Functions on test x.xml</t>
   </si>
   <si>
-    <t>REV 4</t>
+    <t>V.4</t>
   </si>
   <si>
     <t>20171227</t>
@@ -391,7 +391,7 @@
     <t>Converted to openpyxl</t>
   </si>
   <si>
-    <t>REV 5</t>
+    <t>V.5</t>
   </si>
   <si>
     <t>20180112</t>
@@ -400,7 +400,7 @@
     <t>Killed trackvia full table</t>
   </si>
   <si>
-    <t>REV 6</t>
+    <t>V.6</t>
   </si>
   <si>
     <t>20180123</t>
@@ -409,7 +409,7 @@
     <t>Added chinese and auto launch for PIP</t>
   </si>
   <si>
-    <t>REV 7</t>
+    <t>V.7</t>
   </si>
   <si>
     <t>20180223</t>
@@ -418,7 +418,7 @@
     <t>About done</t>
   </si>
   <si>
-    <t>REV 8</t>
+    <t>V.8</t>
   </si>
   <si>
     <t>20180228</t>
@@ -427,7 +427,7 @@
     <t>Migrated to Python3.6.4</t>
   </si>
   <si>
-    <t>REV 9</t>
+    <t>V.9</t>
   </si>
   <si>
     <t>20180307</t>
@@ -436,7 +436,7 @@
     <t>Test build with cx_Freeze5.1.1</t>
   </si>
   <si>
-    <t>REV x.x</t>
+    <t>V.x</t>
   </si>
   <si>
     <t xml:space="preserve">Fiat justitia ruat caelum </t>
@@ -1079,7 +1079,7 @@
         <v>76</v>
       </c>
       <c r="BA2" s="2" t="n">
-        <v>43166.75561099128</v>
+        <v>43167.48612357685</v>
       </c>
     </row>
   </sheetData>
@@ -1101,7 +1101,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="10.8"/>
+    <col customWidth="1" max="1" min="1" width="6"/>
     <col customWidth="1" max="2" min="2" width="12"/>
     <col customWidth="1" max="3" min="3" width="46.8"/>
     <col customWidth="1" max="4" min="4" width="7.199999999999999"/>
@@ -1252,7 +1252,7 @@
         <v>108</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>43166.75549595193</v>
+        <v>43167.4860474883</v>
       </c>
       <c r="C11" t="s">
         <v>109</v>

</xml_diff>

<commit_message>
Test bikes and Ellipticals
</commit_message>
<xml_diff>
--- a/python3.6/PIP_GEN_id-0/Parts - Consoles.xlsx
+++ b/python3.6/PIP_GEN_id-0/Parts - Consoles.xlsx
@@ -180,21 +180,31 @@
     <t>控制台 console</t>
   </si>
   <si>
-    <t>393342</t>
-  </si>
-  <si>
-    <t>ETFM39818</t>
-  </si>
-  <si>
-    <t>TREADMILL_DEVICE</t>
-  </si>
-  <si>
-    <t>OFENDER_DISPLAY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">将电源线连接到EQF1259，将EQW1053的一端连接到EQF1259（CLUB）。注意：请确保您选择与控制台类型相匹配的正确端口。将地线（绿色）连接到E-GND EQF 1259.设置夹具配置：使用PC，在控制台名称（例如：... RNDFtp \ EBNT02117 \ Procedure）下载入RNDftp中的.xml配置文件到microSD卡，将microSD卡正面朝上插入microSD打开灯具背面的RESET按钮，使用UP和DOWN按钮找到合适的配置文件，按ENTER键选择配置文件（屏幕1），等待5秒钟，屏幕稳定后设置灯具脉冲：按下EQF1259 2x上的显示按下此灯具上的开始使用上下按钮设置一个随机脉冲，按下灯具上的开始，按下显示一次。
+    <t>375073</t>
+  </si>
+  <si>
+    <t>ETNT14215</t>
+  </si>
+  <si>
+    <t>INCLINE_TRAINER_DEVICE</t>
+  </si>
+  <si>
+    <t>PM210_DISPLAY_GIBSON_NORDIC</t>
+  </si>
+  <si>
+    <t>“EQF1259控制台夹具
+PC w /访问RNDftp
+MicroSD卡“
+EQW1001; 8针线束
+EQF1259 Console Fixture
+PC w/ Access to RNDftp
+MicroSD Card
+EQW1001; 8-pin harness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“将电源线连接到EQF1259，将EQW1001的一端连接到EQF1259（TRED1）。注意：请确保您选择与控制台类型相匹配的正确端口。将地线（绿色）连接到E-GND EQF 1259.设置夹具配置：使用PC，在控制台名称（例如：... RNDFtp \ EBNT02117 \ Procedure）下载入RNDftp中的.xml配置文件到microSD卡，将microSD卡正面朝上插入microSD打开灯具背面的RESET按钮，使用UP和DOWN按钮找到合适的配置文件，按ENTER键选择配置文件（屏幕1），等待5秒钟，屏幕稳定后设置灯具脉冲：按下EQF1259 2x上的显示按下此灯具上的开始使用上下按钮设置一个随机脉冲，按下灯具上的开始，按下显示一次。
 Connect the power cord to the EQF1259. 
-Connect one end of the EQW1053 to EQF1259 (CLUB). NOTE: MAKE SURE YOU SELECT THE CORRECT PORT THAT MATCH THE TYPE OF THE CONSOLE.   
+Connect one end of the EQW1001 to EQF1259 (TRED1). NOTE: MAKE SURE YOU SELECT THE CORRECT PORT THAT MATCH THE TYPE OF THE CONSOLE.   
 Connect the ground wire (Green) to E-GND on EQF 1259. 
 Set Fixture Configurations:
 Using PC, load .xml configuration file, which is found in the RNDftp under the console name (Example: …RNDFtp\EBNT02117\Procedure) to the microSD card.
@@ -227,60 +237,47 @@
 </t>
   </si>
   <si>
-    <t>将14针MTA连接到控制台。在EQF1259上，打开控制台电源开关。
-Connect the 14-pin MTA to console. On the EQF1259, turn on the Console power switch.</t>
+    <t>将8针MTA连接到控制台。在EQF1259上，打开控制台电源开关。
+Connect the 8-pin MTA to console. On the EQF1259, turn on the Console power switch.</t>
   </si>
   <si>
     <t>将死者的钥匙插入控制台。
 Insert Dead Man Key into console.</t>
   </si>
   <si>
-    <t xml:space="preserve">“在插入SAFETY键时按下STOP按钮。
-按三次STOP键查看软件。
-验证并记录显示在屏幕上的软件版本V80.262或更高版本。
-按SPEED ^按钮确认并记录OLY 73屏幕上显示的OLYMPUS开发板软件版本。
-按SPEED ^按钮验证并记录显示在屏幕上的Wahoo板软件版本，W 1.13.1。
-按SPEED ^按钮以验证并记录屏幕上显示的Bootloader软件版本，3.1.4.5。
-按SPEED ^按钮确认并记录屏幕上显示的USB软件版本USB22。
-按SPEED ^按钮以验证屏幕上显示的序列号。 它应该与序列号标签上的序列号相同。
-拉安全钥匙返回到欢迎光临橙色理论屏幕。“
-Press the STOP button while inserting the SAFETY Key.
-Press STOP three times to view software.
-Verify and record the software version V80.262 or greater showing on the screen.
-Press SPEED ^ button to verify and record the OLYMPUS board software version showing on the screen, OLY 73. 
-Press SPEED ^ button to verify and record the Wahoo board software version showing on the screen, W 1.13.1. 
-Press SPEED ^ button to verify and record the Bootloader software version showing on the screen, 3.1.4.5.
-Press SPEED ^ button to verify and record the USB software version showing on the screen, USB22.
-Press SPEED ^ button to verify the Serial Number showing on the screen. It should be the same as the serial number on the serial number sticker. 
-Pull safety key to return to the WELCOME TO ORANGE THEORY screen.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">插入SAFETY键时按STOP按钮。
-按停止，屏幕将显示“按下或按下校准”。
-按INCLINE ^校准斜面。
-拉安全钥匙返回到欢迎光临橙色理论屏幕。
-Press the STOP button while inserting the SAFETY Key.
-Press STOP, the screen will show “PRESS INCLINE UP OR DOWN TO CALIBRATE”.
-Press the INCLINE ^ to calibrate the incline. 
-Pull safety key to return to the WELCOME TO ORANGE THEORY screen.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">“在插入SAFETY键时按下STOP按钮。
-按STOP两次，看到屏幕上显示的“OTF SYNC”。
-OTF SYNC LED将打开，然后所有其他LED将打开和关闭。 使用SPEED ^使此过程更快。
-拉安全钥匙返回到欢迎光临橙色理论屏幕。“
-Press the STOP button while inserting the SAFETY Key.
-Press STOP two times to see the “OTF SYNC” showing on the screen.
-OTF SYNC LED will turn on, and then all the other LED will turn on and off. Use SPEED ^ to make this process quicker.
-Pull safety key to return to the WELCOME TO ORANGE THEORY screen.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">“插入SAFETY键时按STOP按钮，确认语言为英文，使用SPEED ^改变英文和公制之间的语言。
-按下停止按钮六次，然后按下所有其他按钮，以验证屏幕上显示的联合密钥代码。 注意：每个按钮应显示一个唯一的代码。 如果没有，或者按下按钮难以获得显示，则拒绝控制台。
-拉安全钥匙返回到欢迎光临橙色理论屏幕。“
-Press the STOP button while inserting the SAFETY Key. Verify the language is ENGLISH. Use SPEED ^ to change the language between ENGLISH and METRIC. 
-Press the STOP button six times and then all the other buttons to verify the union Keycode showing on the screen. NOTE: Every button should display a unique code. If it does not or it is difficult to get a display from the button press, reject console.
-Pull safety key to return to the WELCOME TO ORANGE THEORY screen.  </t>
+    <t xml:space="preserve">“按iFIT同步按钮，在显示屏中间验证一个4字符的十六进制（例如：”DF69“）。点击平板电脑屏幕右上方的蓝牙图标在弹出的窗口中，点击您的机器选择并验证信号点击“确定”，平板显示器右上方的蓝牙图标将闪烁，然后变为蓝色，控制台将显示连接指示灯，点击右上角的蓝牙图标平板电脑屏幕和“UNPAIR”控制台。
+Press the iFIT sync button and verify a 4 character Hex in the middle of the display (Example: “DF69”). 
+Tap the Bluetooth icon on the top right of tablet screen
+In the pop up window, tap your machine choice and verify signal strength at 0.5m is (&gt;50%)
+Tap “OKAY”. The Bluetooth icon in the upper right of the tablet display will blink and then go solid blue. The console will show connection indicator.
+Tap the Bluetooth icon on the upper right on tablet screen and “UNPAIR” the console.
+</t>
+  </si>
+  <si>
+    <t>按“”设置“”或“齿轮”图标按钮
+验证和记录“。
+Press the "SETTINGS" or Gear icon button
+Verify and Record.</t>
+  </si>
+  <si>
+    <t>按“”设置“”或“齿轮”图标按钮
+按下按钮两次
+按两次按钮清除并填充所有的段
+确认没有LCD部分应该是暗淡的，丢失，重影，发光或熄灭。“
+Press the "SETTINGS" or Gear icon button
+Press the ˄ button two times
+Press some button two times to clear and fill all segments
+Verify that there are no LCD segments should be dim, missing, ghosting, aglow, or out.</t>
+  </si>
+  <si>
+    <t>按“”设置“”或“齿轮”图标按钮
+按下按钮三次
+按控制台上的所有按钮，每个按钮都将显示一个唯一的代码
+按下按钮返回主屏幕“
+Press the "SETTINGS" or Gear icon button
+Press the ˄ button three times
+Press all the buttons on the console and each will display a unique code
+Press the ˄ button to  return to main screen</t>
   </si>
   <si>
     <t>“在控制台上，按随机快速按钮。
@@ -295,43 +292,35 @@
 Verify that the Incline on the console and EQF1259 match.</t>
   </si>
   <si>
-    <t>将EQF1259的USB电缆插入控制台，并确认EQF1259上显示“USB”。
-Plug USB cable from EQF1259 into console and verify "USB" is displayed on the EQF1259.</t>
-  </si>
-  <si>
     <t>保持脉冲条并确认显示脉冲读数
 Hold the pulse bars and verify a pulse reading is displayed</t>
   </si>
   <si>
-    <t>用拇指轻轻摩擦传感器，显示心率
+    <t>按显示按钮转到BLE脉冲屏幕。
+按开始按钮。
+点击控制台上的IFIT同步按钮。
+验证在控制台上读取脉冲BLE脉冲。
+Press Display button to goto BLE Pulse screen.
+Press Start button.
 Run manual workout on the console.
-Gently rub the sensors with your thumbs will a heart rate displays</t>
-  </si>
-  <si>
-    <t>“将3针风扇连接到控制台。
-在控制台上，按大风扇按钮打开风扇。 球迷应该跑低。
+Tap the IFIT sync button on the console.
+Verify pulse BLE pulse is read on console.</t>
+  </si>
+  <si>
+    <t>“在控制台上，按大风扇按钮打开风扇，风扇应该低速运行。
 再次按大风扇按钮，风扇应该运行在高位。
 按小风扇按钮将风扇转到低位，然后再次按下以关闭风扇。“
-Connect the 3-pin fans to the console.
 On the console, press the Large Fan button to turn fan on. Fan should run on low.
 Press the Large Fan button again and the fan should run on high.
 Press the Small Fan button to turn fan to low, then press again to turn fan off.</t>
   </si>
   <si>
-    <t>“将视频源连接到MYE电视
-将EQWxxxx公头直流电源连接至公头直流电源适配器电缆至MYE电视机，另一端连接至控制台背面
-将RJ45以太网电缆的一端连接到MYE电视机，另一端连接到控制台的背面
-将耳机连接到控制台并放置在耳朵上
-使用控制台控制开启电视机，并在MYE电视机上播放视频源
-音频将通过耳机播放
-在调音台上调节电视音量，此功能将显示在MYE电视上，耳机音频将反映变化“
-Connect analog video source to MYE TV
-Connect EQWxxxx male dc to male dc power adapter cable to MYE TV and other end to back of console
-Connect one end of RJ45 ethernet cable to the MYE TV and other end to back of console
-Connect headphones to console and place on ears
-Turn on TV with console controls and play video source on MYE TV
-Audio will play through the headphones
-Adjust TV audio volume on console and the function will display on the MYE TV and the headphone audio will reflect change</t>
+    <t>“将EQW1007连接到iOS音频源，并将EQW1007的另一端连接到控制台。
+播放音频并验证它是否从控制台扬声器播放。
+调整音量到最低和最高水平，并验证一个变化。“
+Connect the EQW1007 to the iOS audio source and connect the other end of the EQW1007 to the console.
+Play audio and verify that it plays out of the console speakers.
+Adjust the volume to minimum and maximum level and verify a change.</t>
   </si>
   <si>
     <t>“在EQF1259上，关闭控制台电源。
@@ -478,9 +467,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -1021,43 +1013,44 @@
       <c r="G2" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="I2" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG2" s="1" t="s">
-        <v>65</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="AG2" s="1" t="s"/>
       <c r="AH2" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AJ2" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AL2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AO2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AP2" s="1" t="s">
         <v>70</v>
       </c>
       <c r="AQ2" s="1" t="s">
@@ -1069,17 +1062,17 @@
       <c r="AS2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AU2" s="1" t="s">
+      <c r="AT2" s="1" t="s">
         <v>74</v>
       </c>
       <c r="AW2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AY2" t="s">
+      <c r="AY2" s="1" t="s">
         <v>76</v>
       </c>
       <c r="BA2" s="2" t="n">
-        <v>43172.43361110571</v>
+        <v>43173.69217722318</v>
       </c>
     </row>
   </sheetData>
@@ -1251,8 +1244,8 @@
       <c r="A11" t="s">
         <v>108</v>
       </c>
-      <c r="B11" s="2" t="n">
-        <v>43172.43354316771</v>
+      <c r="B11" s="3" t="n">
+        <v>43173.69209976173</v>
       </c>
       <c r="C11" t="s">
         <v>109</v>

</xml_diff>

<commit_message>
updated pbvr and pip_gen
</commit_message>
<xml_diff>
--- a/python3.6/PIP_GEN_id-0/Parts - Consoles.xlsx
+++ b/python3.6/PIP_GEN_id-0/Parts - Consoles.xlsx
@@ -180,10 +180,10 @@
     <t>控制台 console</t>
   </si>
   <si>
-    <t>398332</t>
-  </si>
-  <si>
-    <t>ETNT17217V1</t>
+    <t>405368</t>
+  </si>
+  <si>
+    <t>ETNT24019</t>
   </si>
   <si>
     <t>TREADMILL_DEVICE</t>
@@ -317,11 +317,9 @@
 Verify pulse BLE pulse is read on console.</t>
   </si>
   <si>
-    <t>“将3针风扇连接到控制台。
-在控制台上，按大风扇按钮打开风扇。 球迷应该跑低。
+    <t>“在控制台上，按大风扇按钮打开风扇，风扇应该低速运行。
 再次按大风扇按钮，风扇应该运行在高位。
 按小风扇按钮将风扇转到低位，然后再次按下以关闭风扇。“
-Connect the 3-pin fans to the console.
 On the console, press the Large Fan button to turn fan on. Fan should run on low.
 Press the Large Fan button again and the fan should run on high.
 Press the Small Fan button to turn fan to low, then press again to turn fan off.</t>
@@ -1127,7 +1125,7 @@
         <v>77</v>
       </c>
       <c r="BA2" s="2" t="n">
-        <v>43234.37931664426</v>
+        <v>43383.40542136635</v>
       </c>
     </row>
   </sheetData>
@@ -1342,7 +1340,7 @@
         <v>118</v>
       </c>
       <c r="B14" s="3" t="n">
-        <v>43234.37914697296</v>
+        <v>43383.40522267423</v>
       </c>
       <c r="C14" t="s">
         <v>119</v>

</xml_diff>

<commit_message>
Logged some more cy101
</commit_message>
<xml_diff>
--- a/python3.6/PIP_GEN_id-0/Parts - Consoles.xlsx
+++ b/python3.6/PIP_GEN_id-0/Parts - Consoles.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Parts - Consoles" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="125">
   <si>
     <t>RecordID</t>
   </si>
@@ -180,38 +180,22 @@
     <t>控制台 console</t>
   </si>
   <si>
-    <t>398232</t>
-  </si>
-  <si>
-    <t>ERWNT99147V1</t>
-  </si>
-  <si>
-    <t>ROWER_DEVICE</t>
-  </si>
-  <si>
-    <t>CD_DISPLAY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“将电源线连接到EQF1259。
-将EQW1139的一端连接到EQF1259（BIKE1）。 注：请确保您选择与控制台类型相匹配的正确端口。
-将VDC适配器的一端连接到EQF1259上的“”CONSOLE“”插孔
-设置夹具配置：
-使用PC，在控制台名称下（例如：... RNDFtp \ EBNT02117 \ Procedure），在RNDftp中加载.xml配置文件到microSD卡。
-将microSD卡正面朝上插入microSD卡插槽。
-打开灯具背面的RESET按钮。
-使用UP和DOWN按钮找到正确的配置文件。
-按ENTER键选择配置文件（屏幕1）。
-等待5秒钟，屏幕稳定如下。
-设置灯具脉冲：
-按下EQF1259 2x上的显示。
-按下此灯具上的开始
-使用向上和向下按钮，设置一个随机脉冲。
-按下夹具上的开始。
-按一次显示。
-“
+    <t>391863</t>
+  </si>
+  <si>
+    <t>EKFM74817</t>
+  </si>
+  <si>
+    <t>TREADMILL_DEVICE</t>
+  </si>
+  <si>
+    <t>NO_DISPLAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">将电源线连接到EQF1259，将EQW1053的一端连接到EQF1259（CLUB）。注意：请确保您选择与控制台类型相匹配的正确端口。将地线（绿色）连接到E-GND EQF 1259.设置夹具配置：使用PC，在控制台名称（例如：... RNDFtp \ EBNT02117 \ Procedure）下载入RNDftp中的.xml配置文件到microSD卡，将microSD卡正面朝上插入microSD打开灯具背面的RESET按钮，使用UP和DOWN按钮找到合适的配置文件，按ENTER键选择配置文件（屏幕1），等待5秒钟，屏幕稳定后设置灯具脉冲：按下EQF1259 2x上的显示按下此灯具上的开始使用上下按钮设置一个随机脉冲，按下灯具上的开始，按下显示一次。
 Connect the power cord to the EQF1259. 
-Connect one end of the EQW1139 to EQF1259 (BIKE1). NOTE: MAKE SURE YOU SELECT THE CORRECT PORT THAT MATCH THE TYPE OF THE CONSOLE.
-Connect one end of the VDC adapter to "CONSOLE" socket on the EQF1259
+Connect one end of the EQW1053 to EQF1259 (CLUB). NOTE: MAKE SURE YOU SELECT THE CORRECT PORT THAT MATCH THE TYPE OF THE CONSOLE.   
+Connect the ground wire (Green) to E-GND on EQF 1259. 
 Set Fixture Configurations:
 Using PC, load .xml configuration file, which is found in the RNDftp under the console name (Example: …RNDFtp\EBNT02117\Procedure) to the microSD card.
 Insert the microSD card face up into the microSD card slot.
@@ -232,120 +216,130 @@
 Verify that the ESD bag is dissipative and it is printed on as per the drawing.</t>
   </si>
   <si>
-    <t xml:space="preserve">“确保设备包装在防静电袋中，目视检查控制台是否有化妆品缺陷，物理损坏和不清晰的打印。
-Ensure the unit is packaged in an antistatic bag. 
-Visually inspect the console for cosmetic defects, physical damage, and illegible printing.  
-Verify console matches picture
-</t>
+    <t>验证是否在控制台或脉冲条上打印了常规警告。
+Verify that the General Warning is printed on the console or pulse bar.</t>
   </si>
   <si>
     <t>“如果需要连接;脉冲条/手柄，扬声器，风扇，电视等。
-将10针MTA连接到控制台。
-如果使用电池测试控制台，请确保在安装电池之前控制台电源开关已关闭，并且电池电压良好。用电池测试一半样品。见警告。
-警告！不要将电池安装到控制台电源开关的控制台上！这可能会导致电池充电和爆炸。
-警告！请勿安装组合电压低于2伏的电池。这可能会导致电池充电和爆炸。
-电池测试：一旦安装了电池，无论控制台开关位置如何，控制台电源指示灯都会亮起，表示控制台已通电。
-打开控制台电源开关时，EQF1259会检查控制台电压线，如果检测到2伏以上，则EQF1259假定控制台由电池供电，并且不打开控制台电压线的电源。屏幕右上角将出现“Bat”字样，EQF1259将向控制台提供信号。
-VDC适配器测试：将VDC适配器连接到控制台
+将14针MTA连接到控制台。
 在EQF1259上，打开控制台电源开关。“
 Connect if needed; pulse bar/grips, speakers, fans, TV, etc.
-Connect the 10-pin MTA to console.
-If testing a console with batteries, be absolutely sure the console power switch is off before installing batteries and that the batteries have a good voltage.   Test half sample with batteries. See warnings. 
-Warning!  DO NOT INSTALL BATTERIES INTO A CONSOLE WITH THE CONSOLE POWER SWITCH ON!  THIS MAY CAUSE BATTERIES TO CHARGE AND EXPLODE.
-Warning!  DO NOT INSTALL BATTERIES THAT HAVE A COMBINED VOLTAGE LESS THAN 2 VOLTS. THIS MAY CAUSE BATTERIES TO CHARGE AND EXPLODE.
-Battery test: Once batteries are installed, the Console Power LED will light regardless of the console switch position indicating the console had power. 
-When turning on the console power switch, the EQF1259 checks the console voltage line and if more than 2 volts is detected, the EQF1259 assumes the console is powered by batteries and does not turn on power to the console voltage wires.  The word “Bat” will appear in the top right corner of the display and the EQF1259 will provide signals to the console.
-VDC adapter test: Connect the VDC adapter to console
+Connect the 14-pin MTA to console.
 On the EQF1259, turn on the Console power switch.</t>
   </si>
   <si>
-    <t xml:space="preserve">如果控制台显示“Hello”或“ifit.com/activate”，请按住iFit（SYNC）按钮10秒钟
-触摸屏幕左上角的用户个人资料图标
-在下拉列表中，触摸蓝牙
-按控制台上的iFIT同步按钮，验证显示屏中间的4字符十六进制代码（例如：“DF69”）。
-在弹出窗口中，验证与4字符十六进制代码匹配的控制台的信号强度为0.5m（&gt; 50％）
-连接到与4个字符的十六进制代码匹配的控制台
-触摸屏幕左上角的用户个人资料图标
-在下拉列表中，触摸蓝牙
-断开与控制台的连接
-If console displays  "Hello" or "ifit.com/activate", press and hold the iFit (SYNC) button for 10 seconds
-Touch user profile icon at the upper left  of the screen
-In drop down list, touch Bluetooth
-Press the iFIT sync button on the console and verify a 4 character hex code in the middle of the display (Example: “DF69”). 
-In the pop up window, verify signal strength of the console that matches the 4 character hex code is at 0.5m is (&gt;50%)
-Connect to the console that matches the 4 character hex code
-Touch user profile icon at the upper left  of the screen
-In drop down list, touch Bluetooth
-Disconnect from console
+    <t>将安全钥匙插入控制台。
+Insert safety key into console.</t>
+  </si>
+  <si>
+    <t>“在屏幕的外边缘绘制一个矩形。
+触摸“”维护“”。 这将显示应用程序版本和Brainboard版本。
+验证和记录。
+按下数位板上的后退箭头返回主屏幕“
+Draw a rectangle around the outer edge of the screen.
+Touch "Maintainance". This will display App version and Brainboard version.
+Verify and Record.
+Press the back arrow on the tablet to return to main screen</t>
+  </si>
+  <si>
+    <t>“在屏幕的外边缘绘制一个矩形
+触摸“”维护“”
+选择校准倾斜
+在EQF1259上按Calibrate
+按开始在平板电脑上开始倾斜校准。 确认显示屏上的倾斜值短暂增加，暂停，然后减小到零
+校准完成后，按下数位板上的后退箭头返回主屏幕“
+Draw a rectangle around the outer edge of the screen
+Touch "Maintainance"
+Select Calibrate Incline
+Press Calibrate on EQF1259
+Press Begin on tablet to start incline calibration.  Verify the incline value on the display increases briefly, pauses, then decrease to zero
+When calibration is complete, press the back arrow on the tablet to return to main screen</t>
+  </si>
+  <si>
+    <t>验证平板电脑显示屏是否亮起且没有缺陷
+Verify tablet display is lit and without flaws</t>
+  </si>
+  <si>
+    <t>“在屏幕的外边缘绘制一个矩形
+触摸“”维护“”
+选择键码
+按控制台上的所有按钮，每个按钮都将显示一个唯一的代码
+按下数位板上的后退箭头返回主屏幕“
+Draw a rectangle around the outer edge of the screen
+Touch "Maintainance"
+Select Keycodes
+Press all the buttons on the console and each will display a unique code
+Press the back arrow on the tablet to return to main screen</t>
+  </si>
+  <si>
+    <t>“在控制台上开始手动锻炼。
+在控制台上，按随机快速按钮。
+验证控制台和EQF1259上的速度是否匹配。“
+Start manual workout on the console.
+On the console, press random Quick speed buttons.
+Verify that the Speed on the console and EQF1259 match.</t>
+  </si>
+  <si>
+    <t>“在控制台上，按随机快速倾斜按钮。
+验证控制台上的倾斜和EQF1259匹配。“
+On the console, press random Quick incline buttons.
+Verify that the Incline on the console and EQF1259 match.</t>
+  </si>
+  <si>
+    <t>将EQF1259的USB电缆插入控制台，并确认EQF1259上显示“USB”。
+Plug USB cable from EQF1259 into console and verify "USB" is displayed on the EQF1259.</t>
+  </si>
+  <si>
+    <t>保持脉冲条并确认显示脉冲读数
+Hold the pulse bars and verify a pulse reading is displayed</t>
+  </si>
+  <si>
+    <t>用拇指轻轻摩擦传感器，显示心率
+Run manual workout on the console.
+Gently rub the sensors with your thumbs will a heart rate displays</t>
+  </si>
+  <si>
+    <t>“在控制台上，按大风扇按钮打开风扇，风扇应该低速运行。
+再次按大风扇按钮，风扇应该运行在高位。
+按小风扇按钮将风扇转到低位，然后再次按下以关闭风扇。“
+On the console, press the Large Fan button to turn fan on. Fan should run on low.
+Press the Large Fan button again and the fan should run on high.
+Press the Small Fan button to turn fan to low, then press again to turn fan off.</t>
+  </si>
+  <si>
+    <t>“将EQF1007的一端连接到音频源，另一端连接到MYE音频发射器
+开启MYE音频发射器并播放音频源
+将耳机连接到控制台
+将MYE音频接收器连接到控制台背面的RJ45电缆
+音频源将通过耳机播放
+调节音量，耳机音频将反映变化“
+Connect one end of EQF1007 to audio source and the other end to MYE audio transmitter
+Power up MYE audio transmitter and play audio source
+Connect headphones to console
+Connect MYE audio receiver to RJ45 cable on the back of console
+Audio source will play through the headphones
+Adjust volume and the headphone audio will reflect change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">将音频源连接到EQF1293并按播放
+将EQWxxxx公头直流电连接到公头直流电源适配器电缆，连接到EQF1293和控制台的其他端到端
+将RJ45以太网电缆的一端连接到EQF1293和控制台的另一端到后端
+将耳机连接到控制台并放在耳朵上
+按下控制台上的所有电视控制按钮，EQF1293上将显示响应
+音频将通过耳机播放
+在控制台上调整电视音频音量，该功能将显示在MYE电视上，耳机音频将反映变化
+Connect audio source to EQF1293 and press play
+Connect EQWxxxx male dc to male dc power adapter cable to EQF1293 and other end to back of console
+Connect one end of RJ45 ethernet cable to the EQF1293 and other end to back of console
+Connect headphones to console and place on ears
+Press all the TV control buttons on the console and a response will appear on the EQF1293
+Audio will play through the headphones
+Adjust TV audio volume on console and the function will display on the MYE TV and the headphone audio will reflect change
 </t>
   </si>
   <si>
-    <t>按“”设置“”或“齿轮”图标按钮
-验证和记录“。
-Press the "SETTINGS" or Gear icon button
-Verify and Record.</t>
-  </si>
-  <si>
-    <t>按“”设置“”或“齿轮”图标按钮
-按下按钮两次
-按两次按钮清除并填充所有的段
-确认没有LCD部分应该是暗淡的，丢失，重影，发光或熄灭。“
-Press the "SETTINGS" or Gear icon button
-Press the ˄ button two times
-Press some button two times to clear and fill all segments
-Verify that there are no LCD segments should be dim, missing, ghosting, aglow, or out.</t>
-  </si>
-  <si>
-    <t>按“”设置“”或“齿轮”图标按钮
-按下按钮三次
-按控制台上的所有按钮，每个按钮都将显示一个唯一的代码
-按下按钮返回主屏幕“
-Press the "SETTINGS" or Gear icon button
-Press the ˄ button three times
-Press all the buttons on the console and each will display a unique code
-Press the ˄ button to  return to main screen</t>
-  </si>
-  <si>
-    <t>“在控制台上开始手动锻炼
-在EQF1259上按START（开始）。
-验证控制台上的Cadence（RPM）和EQF1259匹配。“
-Start manual workout on the console
-On the EQF1259, Press START.
-Verify that the Cadence(RPM) on the console and the EQF1259 match.</t>
-  </si>
-  <si>
-    <t>“在控制台上，按下RESISTANCE +按钮，确认EQF1259的电阻值增加。
-在控制台上，按RESISTANCE - 按钮。 验证EQF1259的电阻值是否下降。“
-On the console, press the RESISTANCE + button. Verify the resistance level on the EQF1259 increases.  
-On the console, press the RESISTANCE - button. Verify the resistance level on the EQF1259 decreases.</t>
-  </si>
-  <si>
-    <t>“在EQF1259上，按显示按钮转到BLE脉冲屏幕。
-按下开始按钮。
-在控制台上运行手动锻炼。
-点击控制台上的IFIT同步按钮。
-验证在控制台上读取脉冲BLE脉冲。“
-On the EQF1259, press Display button to goto BLE Pulse screen.
-Press Start button.
-Run manual workout on the console.
-Tap the IFIT sync button on the console.
-Verify pulse BLE pulse is read on console.</t>
-  </si>
-  <si>
-    <t>“将EQW1007连接到iOS音频源，并将EQW1007的另一端连接到控制台。
-播放音频并验证它是否从控制台扬声器播放。
-调整音量到最低和最高水平，并验证一个变化。“
-Connect the EQW1007 to the iOS audio source and connect the other end of the EQW1007 to the console.
-Play audio and verify that it plays out of the console speakers.
-Adjust the volume to minimum and maximum level and verify a change.</t>
-  </si>
-  <si>
-    <t>“按下并按住Ifit按钮（同步）并且速度增加和减少3秒钟以锁定控制台
-验证是否显示“”Hello“”或“”ifit.com/activate“”
-在EQF1259上，关闭控制台电源。
+    <t>“在EQF1259上，关闭控制台电源。
 断开控制台上的所有电线和电缆。“
-Lock console by press and holding the Ifit button (SYNC) and the Speed increase and decrease for 3 seconds
-Verify that "Hello" or "ifit.com/activate" is displayed
 On the EQF1259, turn off the Console power.
 Disconnect all wires and cables from the console.</t>
   </si>
@@ -1085,45 +1079,59 @@
       <c r="S2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>60</v>
       </c>
       <c r="Z2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>62</v>
       </c>
       <c r="AE2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AG2" s="1" t="s"/>
+      <c r="AG2" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="AH2" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AJ2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AM2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AN2" s="1" t="s">
+      <c r="AL2" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="AO2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="AR2" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
+      </c>
+      <c r="AS2" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="AT2" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
+      </c>
+      <c r="AU2" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="AW2" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="AY2" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="BA2" s="2" t="n">
-        <v>43451.48887678594</v>
+        <v>43474.60679079696</v>
       </c>
     </row>
   </sheetData>
@@ -1153,226 +1161,226 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D4" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="D5" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C6" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D6" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C7" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D7" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="D8" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C9" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D9" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B10" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D10" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="B11" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C11" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D11" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B12" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C12" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="D12" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B13" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C13" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D13" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="B14" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="C14" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="D14" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="B15" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="C15" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="D15" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B16" s="3" t="n">
-        <v>43451.4888292622</v>
+        <v>43474.60642766125</v>
       </c>
       <c r="C16" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="D16" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>